<commit_message>
feat: Grundlagen Kapitel umstrukturiert, 04_02 erwietert und Excel Mapping Study erweiter
</commit_message>
<xml_diff>
--- a/Excel/Mapping Study.xlsx
+++ b/Excel/Mapping Study.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="480" documentId="13_ncr:1_{4E6D62AD-4014-C54F-8508-75C30E73A565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BB6758B-882F-496A-ACB2-8AAC405539E0}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{0DD4CFEA-C2F1-46F7-88F8-AB6F3727EE8E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{0DD4CFEA-C2F1-46F7-88F8-AB6F3727EE8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Zusammenfassung RQ1" sheetId="1" r:id="rId1"/>
@@ -427,20 +427,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -867,7 +867,7 @@
       </c>
     </row>
     <row r="2" spans="1:46" s="4" customFormat="1" ht="51.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="27" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -923,7 +923,7 @@
       <c r="AT2"/>
     </row>
     <row r="3" spans="1:46" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A3" s="24"/>
+      <c r="A3" s="27"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -977,7 +977,7 @@
       <c r="AT3"/>
     </row>
     <row r="4" spans="1:46" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="24"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1031,7 +1031,7 @@
       <c r="AT4"/>
     </row>
     <row r="5" spans="1:46" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A5" s="24"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1085,7 +1085,7 @@
       <c r="AT5"/>
     </row>
     <row r="6" spans="1:46" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A6" s="24"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1139,7 +1139,7 @@
       <c r="AT6"/>
     </row>
     <row r="7" spans="1:46" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.35">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="27" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1195,7 +1195,7 @@
       <c r="AT7"/>
     </row>
     <row r="8" spans="1:46" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="24"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1249,7 +1249,7 @@
       <c r="AT8"/>
     </row>
     <row r="9" spans="1:46" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A9" s="24"/>
+      <c r="A9" s="27"/>
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1303,7 +1303,7 @@
       <c r="AT9"/>
     </row>
     <row r="10" spans="1:46" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A10" s="24"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
@@ -1357,7 +1357,7 @@
       <c r="AT10"/>
     </row>
     <row r="11" spans="1:46" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.35">
-      <c r="A11" s="24"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
@@ -1423,8 +1423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77FA32D9-5FDF-4B13-A8A2-A3E26E74C01B}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1562,8 +1562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3262B687-1B36-4642-B0C3-0FB5595C7692}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2407,7 +2407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0B9B836-856D-4E27-9EE4-62FFF85FE8A1}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:C8"/>
     </sheetView>
   </sheetViews>
@@ -2460,10 +2460,10 @@
       <c r="A4" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="26">
         <v>13</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C4" s="26">
         <v>10</v>
       </c>
       <c r="D4" s="23">
@@ -2499,31 +2499,31 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2559,7 +2559,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="23">
@@ -2573,7 +2573,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="23">
@@ -2587,13 +2587,13 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="26">
         <v>15</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C4" s="26">
         <v>10</v>
       </c>
       <c r="D4" s="23">
@@ -2601,7 +2601,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>40</v>
       </c>
       <c r="B5" s="23">
@@ -2615,7 +2615,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="24" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="23">
@@ -2629,11 +2629,11 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
feat: Excel und figure 04_01 verbessert
</commit_message>
<xml_diff>
--- a/Excel/Mapping Study.xlsx
+++ b/Excel/Mapping Study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilsarnold/Documents/WIN-Studium/7. Semester/BA/Thesis/Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bosch-my.sharepoint.com/personal/nnr3fe_bosch_com/Documents/PersonalDrive/HTWG/BA/LaTex/Thesis/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA54909-9B0A-EF4B-BA4D-7F07283153F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="6_{1C4991A2-5980-45E5-84EC-2227ABB33033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95418BC8-1A71-4E50-AED8-963159553336}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5" xr2:uid="{0DD4CFEA-C2F1-46F7-88F8-AB6F3727EE8E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="5" xr2:uid="{0DD4CFEA-C2F1-46F7-88F8-AB6F3727EE8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Zusammenfassung RQ1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="93">
   <si>
     <t>Anzahl Papers</t>
   </si>
@@ -714,12 +714,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -734,15 +728,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -789,6 +774,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -797,6 +788,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1204,16 +1204,16 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.6328125" customWidth="1"/>
+    <col min="2" max="2" width="30.6328125" customWidth="1"/>
     <col min="3" max="3" width="39" customWidth="1"/>
-    <col min="4" max="4" width="74.6640625" customWidth="1"/>
-    <col min="5" max="5" width="41.1640625" customWidth="1"/>
+    <col min="4" max="4" width="74.6328125" customWidth="1"/>
+    <col min="5" max="5" width="41.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.35">
       <c r="B1" s="3"/>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -1222,8 +1222,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:46" s="4" customFormat="1" ht="51.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:46" s="4" customFormat="1" ht="51.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="45" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1278,8 +1278,8 @@
       <c r="AS2"/>
       <c r="AT2"/>
     </row>
-    <row r="3" spans="1:46" s="4" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A3" s="23"/>
+    <row r="3" spans="1:46" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A3" s="45"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1332,8 +1332,8 @@
       <c r="AS3"/>
       <c r="AT3"/>
     </row>
-    <row r="4" spans="1:46" s="4" customFormat="1" ht="80" x14ac:dyDescent="0.2">
-      <c r="A4" s="23"/>
+    <row r="4" spans="1:46" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="45"/>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1386,8 +1386,8 @@
       <c r="AS4"/>
       <c r="AT4"/>
     </row>
-    <row r="5" spans="1:46" s="4" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A5" s="23"/>
+    <row r="5" spans="1:46" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A5" s="45"/>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1440,8 +1440,8 @@
       <c r="AS5"/>
       <c r="AT5"/>
     </row>
-    <row r="6" spans="1:46" s="4" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A6" s="23"/>
+    <row r="6" spans="1:46" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6" s="45"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1494,8 +1494,8 @@
       <c r="AS6"/>
       <c r="AT6"/>
     </row>
-    <row r="7" spans="1:46" s="4" customFormat="1" ht="96" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
+    <row r="7" spans="1:46" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A7" s="45" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1550,8 +1550,8 @@
       <c r="AS7"/>
       <c r="AT7"/>
     </row>
-    <row r="8" spans="1:46" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A8" s="23"/>
+    <row r="8" spans="1:46" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="45"/>
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1604,8 +1604,8 @@
       <c r="AS8"/>
       <c r="AT8"/>
     </row>
-    <row r="9" spans="1:46" s="4" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A9" s="23"/>
+    <row r="9" spans="1:46" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A9" s="45"/>
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1658,8 +1658,8 @@
       <c r="AS9"/>
       <c r="AT9"/>
     </row>
-    <row r="10" spans="1:46" s="4" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A10" s="23"/>
+    <row r="10" spans="1:46" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A10" s="45"/>
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
@@ -1712,8 +1712,8 @@
       <c r="AS10"/>
       <c r="AT10"/>
     </row>
-    <row r="11" spans="1:46" s="4" customFormat="1" ht="96" x14ac:dyDescent="0.2">
-      <c r="A11" s="23"/>
+    <row r="11" spans="1:46" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A11" s="45"/>
       <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
@@ -1783,13 +1783,13 @@
       <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" customWidth="1"/>
-    <col min="2" max="6" width="21.83203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="32.36328125" customWidth="1"/>
+    <col min="2" max="6" width="21.81640625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>29</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>30</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>34</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>31</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>32</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>33</v>
       </c>
@@ -1922,17 +1922,17 @@
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.83203125" customWidth="1"/>
-    <col min="2" max="2" width="42.5" style="11" customWidth="1"/>
-    <col min="3" max="3" width="27.83203125" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="19.5" style="12" customWidth="1"/>
-    <col min="6" max="10" width="21.83203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="45.81640625" customWidth="1"/>
+    <col min="2" max="2" width="42.453125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="27.81640625" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="19.453125" style="12" customWidth="1"/>
+    <col min="6" max="10" width="21.81640625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>30</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>30</v>
       </c>
@@ -1984,7 +1984,7 @@
       </c>
       <c r="G3"/>
     </row>
-    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>30</v>
       </c>
@@ -2002,7 +2002,7 @@
       </c>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>30</v>
       </c>
@@ -2020,7 +2020,7 @@
       </c>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>34</v>
       </c>
@@ -2056,7 +2056,7 @@
       </c>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
@@ -2074,7 +2074,7 @@
       </c>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>34</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>36</v>
       </c>
@@ -2143,7 +2143,7 @@
       </c>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>36</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>36</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>36</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>37</v>
       </c>
@@ -2228,7 +2228,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>37</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>37</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>37</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>37</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>38</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>38</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>38</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>38</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>38</v>
       </c>
@@ -2395,14 +2395,14 @@
       <selection activeCell="B12" sqref="B12:B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="4" width="23.83203125" customWidth="1"/>
-    <col min="7" max="10" width="26.1640625" customWidth="1"/>
+    <col min="2" max="4" width="23.81640625" customWidth="1"/>
+    <col min="7" max="10" width="26.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>44</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
         <v>48</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>49</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>50</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>51</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>64</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="25" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>56</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>59</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="25" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>56</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>59</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="25" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
         <v>60</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>60</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="25" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
         <v>60</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="14" t="s">
         <v>60</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="25" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
         <v>58</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
         <v>58</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="28" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="25" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="s">
         <v>58</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="14" t="s">
         <v>58</v>
       </c>
@@ -2767,12 +2767,12 @@
       <selection activeCell="A8" sqref="A8:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="29.83203125" customWidth="1"/>
+    <col min="1" max="5" width="29.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4"/>
       <c r="B1" s="17" t="s">
         <v>56</v>
@@ -2784,7 +2784,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>30</v>
       </c>
@@ -2798,7 +2798,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>34</v>
       </c>
@@ -2812,7 +2812,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>31</v>
       </c>
@@ -2826,7 +2826,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>32</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>33</v>
       </c>
@@ -2854,29 +2854,29 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+    <row r="8" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -2893,333 +2893,341 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75DD1D88-089A-304B-8F89-0474B1D6BA35}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="6" width="19.6640625" style="47" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="3.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.6328125" customWidth="1"/>
+    <col min="4" max="6" width="19.6328125" style="42" customWidth="1"/>
+    <col min="7" max="7" width="19.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="50" t="s">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C1" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="52"/>
-    </row>
-    <row r="2" spans="1:7" s="47" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38" t="s">
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="49"/>
+    </row>
+    <row r="2" spans="1:7" s="42" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="31"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="39" t="s">
+      <c r="G2" s="34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="47" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="31" t="s">
+    <row r="3" spans="1:7" s="42" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="25">
+        <v>7</v>
+      </c>
+      <c r="D3" s="25">
+        <v>12</v>
+      </c>
+      <c r="E3" s="25">
+        <v>11</v>
+      </c>
+      <c r="F3" s="25">
+        <v>12</v>
+      </c>
+      <c r="G3" s="29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="42" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="51"/>
+      <c r="B4" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="36">
         <v>3</v>
       </c>
-      <c r="D3" s="27">
+      <c r="D4" s="36">
+        <v>4</v>
+      </c>
+      <c r="E4" s="36">
+        <v>5</v>
+      </c>
+      <c r="F4" s="36">
+        <v>5</v>
+      </c>
+      <c r="G4" s="37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="42" customFormat="1" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="52"/>
+      <c r="B5" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="26">
+        <v>3</v>
+      </c>
+      <c r="D5" s="26">
         <v>6</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E5" s="26">
+        <v>4</v>
+      </c>
+      <c r="F5" s="26">
+        <v>5</v>
+      </c>
+      <c r="G5" s="30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="42" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="25">
         <v>6</v>
       </c>
-      <c r="F3" s="27">
+      <c r="D6" s="25">
+        <v>8</v>
+      </c>
+      <c r="E6" s="25">
+        <v>8</v>
+      </c>
+      <c r="F6" s="25">
+        <v>8</v>
+      </c>
+      <c r="G6" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="42" customFormat="1" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="52"/>
+      <c r="B7" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="26">
+        <v>3</v>
+      </c>
+      <c r="D7" s="26">
+        <v>4</v>
+      </c>
+      <c r="E7" s="26">
+        <v>4</v>
+      </c>
+      <c r="F7" s="26">
         <v>5</v>
       </c>
-      <c r="G3" s="34">
+      <c r="G7" s="30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="42" customFormat="1" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="40">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" s="47" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="32"/>
-      <c r="B4" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="41">
-        <v>1</v>
-      </c>
-      <c r="D4" s="41">
-        <v>2</v>
-      </c>
-      <c r="E4" s="41">
-        <v>3</v>
-      </c>
-      <c r="F4" s="41">
-        <v>2</v>
-      </c>
-      <c r="G4" s="42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="47" customFormat="1" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
-      <c r="B5" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="28">
-        <v>1</v>
-      </c>
-      <c r="D5" s="28">
+      <c r="D8" s="40">
+        <v>6</v>
+      </c>
+      <c r="E8" s="40">
+        <v>7</v>
+      </c>
+      <c r="F8" s="40">
+        <v>5</v>
+      </c>
+      <c r="G8" s="41">
         <v>4</v>
       </c>
-      <c r="E5" s="28">
-        <v>3</v>
-      </c>
-      <c r="F5" s="28">
-        <v>3</v>
-      </c>
-      <c r="G5" s="35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="47" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" s="27">
-        <v>2</v>
-      </c>
-      <c r="D6" s="27">
-        <v>3</v>
-      </c>
-      <c r="E6" s="27">
-        <v>3</v>
-      </c>
-      <c r="F6" s="27">
-        <v>3</v>
-      </c>
-      <c r="G6" s="34">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="47" customFormat="1" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
-      <c r="B7" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="28">
-        <v>1</v>
-      </c>
-      <c r="D7" s="28">
-        <v>2</v>
-      </c>
-      <c r="E7" s="28">
-        <v>2</v>
-      </c>
-      <c r="F7" s="28">
-        <v>2</v>
-      </c>
-      <c r="G7" s="35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="47" customFormat="1" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="44" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="45">
-        <v>2</v>
-      </c>
-      <c r="D8" s="45">
-        <v>2</v>
-      </c>
-      <c r="E8" s="45">
-        <v>2</v>
-      </c>
-      <c r="F8" s="45">
-        <v>1</v>
-      </c>
-      <c r="G8" s="46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="48"/>
-    </row>
-    <row r="10" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="48"/>
-      <c r="B10" s="26" t="s">
+    </row>
+    <row r="9" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="43"/>
+    </row>
+    <row r="10" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="43"/>
+      <c r="B10" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="44" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="48"/>
-      <c r="B11" s="26" t="s">
+    <row r="11" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="43"/>
+      <c r="B11" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="44" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="26" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B12" s="24" t="s">
         <v>73</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B13" s="26" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B13" s="24" t="s">
         <v>74</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="26" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B14" s="24" t="s">
         <v>75</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="26" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B15" s="24" t="s">
         <v>76</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="26" t="s">
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B16" s="24" t="s">
         <v>77</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="26" t="s">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" s="24" t="s">
         <v>78</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="26" t="s">
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B18" s="24" t="s">
         <v>79</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="26" t="s">
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B19" s="24" t="s">
         <v>80</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="26" t="s">
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B20" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="12"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="26" t="s">
+      <c r="C20" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B21" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="12"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="26" t="s">
+      <c r="C21" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B22" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="C22" s="12"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B23" s="26" t="s">
+      <c r="C22" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B23" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="12"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B24" s="26" t="s">
+      <c r="C23" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B24" s="24" t="s">
         <v>85</v>
       </c>
       <c r="C24" s="12"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B25" s="26" t="s">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B25" s="24" t="s">
         <v>86</v>
       </c>
       <c r="C25" s="12"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="26" t="s">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B26" s="24" t="s">
         <v>87</v>
       </c>
       <c r="C26" s="12"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="26" t="s">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B27" s="24" t="s">
         <v>88</v>
       </c>
       <c r="C27" s="12"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="26" t="s">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B28" s="24" t="s">
         <v>89</v>
       </c>
       <c r="C28" s="12"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B29" s="26" t="s">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B29" s="24" t="s">
         <v>90</v>
       </c>
       <c r="C29" s="12"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B30" s="26" t="s">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B30" s="24" t="s">
         <v>91</v>
       </c>
       <c r="C30" s="12"/>
@@ -3243,12 +3251,12 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="30.83203125" customWidth="1"/>
+    <col min="1" max="4" width="30.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4"/>
       <c r="B1" s="17" t="s">
         <v>56</v>
@@ -3260,7 +3268,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
         <v>13</v>
       </c>
@@ -3274,7 +3282,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
         <v>14</v>
       </c>
@@ -3288,7 +3296,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="22" t="s">
         <v>39</v>
       </c>
@@ -3302,7 +3310,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
         <v>40</v>
       </c>
@@ -3316,7 +3324,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="22" t="s">
         <v>41</v>
       </c>
@@ -3330,12 +3338,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="24" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B8" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
feat: kapitel 04_02_03 erweitert
</commit_message>
<xml_diff>
--- a/Excel/Mapping Study.xlsx
+++ b/Excel/Mapping Study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilsarnold/Documents/WIN-Studium/7. Semester/BA/Thesis/Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bosch-my.sharepoint.com/personal/nnr3fe_bosch_com/Documents/PersonalDrive/HTWG/BA/LaTex/Thesis/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21382048-7FF6-864D-B436-643A7D7F9E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="7" xr2:uid="{0DD4CFEA-C2F1-46F7-88F8-AB6F3727EE8E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{0DD4CFEA-C2F1-46F7-88F8-AB6F3727EE8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Zusammenfassung RQ1" sheetId="1" r:id="rId1"/>
@@ -779,6 +779,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -801,15 +810,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1151,16 +1151,16 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.6328125" customWidth="1"/>
+    <col min="2" max="2" width="30.6328125" customWidth="1"/>
     <col min="3" max="3" width="39" customWidth="1"/>
-    <col min="4" max="4" width="74.6640625" customWidth="1"/>
-    <col min="5" max="5" width="41.1640625" customWidth="1"/>
+    <col min="4" max="4" width="74.6328125" customWidth="1"/>
+    <col min="5" max="5" width="41.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.35">
       <c r="B1" s="3"/>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -1169,8 +1169,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:46" s="4" customFormat="1" ht="51.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
+    <row r="2" spans="1:46" s="4" customFormat="1" ht="51.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="43" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1225,8 +1225,8 @@
       <c r="AS2"/>
       <c r="AT2"/>
     </row>
-    <row r="3" spans="1:46" s="4" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A3" s="40"/>
+    <row r="3" spans="1:46" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A3" s="43"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1279,8 +1279,8 @@
       <c r="AS3"/>
       <c r="AT3"/>
     </row>
-    <row r="4" spans="1:46" s="4" customFormat="1" ht="80" x14ac:dyDescent="0.2">
-      <c r="A4" s="40"/>
+    <row r="4" spans="1:46" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="43"/>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1333,8 +1333,8 @@
       <c r="AS4"/>
       <c r="AT4"/>
     </row>
-    <row r="5" spans="1:46" s="4" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A5" s="40"/>
+    <row r="5" spans="1:46" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A5" s="43"/>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1387,8 +1387,8 @@
       <c r="AS5"/>
       <c r="AT5"/>
     </row>
-    <row r="6" spans="1:46" s="4" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A6" s="40"/>
+    <row r="6" spans="1:46" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6" s="43"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1441,8 +1441,8 @@
       <c r="AS6"/>
       <c r="AT6"/>
     </row>
-    <row r="7" spans="1:46" s="4" customFormat="1" ht="96" x14ac:dyDescent="0.2">
-      <c r="A7" s="40" t="s">
+    <row r="7" spans="1:46" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A7" s="43" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1497,8 +1497,8 @@
       <c r="AS7"/>
       <c r="AT7"/>
     </row>
-    <row r="8" spans="1:46" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A8" s="40"/>
+    <row r="8" spans="1:46" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="43"/>
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1551,8 +1551,8 @@
       <c r="AS8"/>
       <c r="AT8"/>
     </row>
-    <row r="9" spans="1:46" s="4" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A9" s="40"/>
+    <row r="9" spans="1:46" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A9" s="43"/>
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1605,8 +1605,8 @@
       <c r="AS9"/>
       <c r="AT9"/>
     </row>
-    <row r="10" spans="1:46" s="4" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A10" s="40"/>
+    <row r="10" spans="1:46" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A10" s="43"/>
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
@@ -1659,8 +1659,8 @@
       <c r="AS10"/>
       <c r="AT10"/>
     </row>
-    <row r="11" spans="1:46" s="4" customFormat="1" ht="96" x14ac:dyDescent="0.2">
-      <c r="A11" s="40"/>
+    <row r="11" spans="1:46" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A11" s="43"/>
       <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
@@ -1730,13 +1730,13 @@
       <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" customWidth="1"/>
-    <col min="2" max="6" width="21.83203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="32.36328125" customWidth="1"/>
+    <col min="2" max="6" width="21.81640625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>29</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>30</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>34</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>31</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>32</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>33</v>
       </c>
@@ -1869,17 +1869,17 @@
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.83203125" customWidth="1"/>
-    <col min="2" max="2" width="42.5" style="11" customWidth="1"/>
-    <col min="3" max="3" width="27.83203125" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="19.5" style="12" customWidth="1"/>
-    <col min="6" max="10" width="21.83203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="45.81640625" customWidth="1"/>
+    <col min="2" max="2" width="42.453125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="27.81640625" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="19.453125" style="12" customWidth="1"/>
+    <col min="6" max="10" width="21.81640625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>30</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>30</v>
       </c>
@@ -1931,7 +1931,7 @@
       </c>
       <c r="G3"/>
     </row>
-    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>30</v>
       </c>
@@ -1949,7 +1949,7 @@
       </c>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>30</v>
       </c>
@@ -1967,7 +1967,7 @@
       </c>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>34</v>
       </c>
@@ -2003,7 +2003,7 @@
       </c>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
@@ -2021,7 +2021,7 @@
       </c>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>34</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>36</v>
       </c>
@@ -2090,7 +2090,7 @@
       </c>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>36</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>36</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>36</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>37</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>37</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>37</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>37</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>37</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>38</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>38</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>38</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>38</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>38</v>
       </c>
@@ -2342,14 +2342,14 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="4" width="23.83203125" customWidth="1"/>
-    <col min="7" max="10" width="26.1640625" customWidth="1"/>
+    <col min="2" max="4" width="23.81640625" customWidth="1"/>
+    <col min="7" max="10" width="26.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>44</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
         <v>48</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>49</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>50</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>51</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>64</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="25" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>56</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>59</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="25" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>56</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>59</v>
       </c>
@@ -2564,7 +2564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="25" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
         <v>60</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>60</v>
       </c>
@@ -2598,7 +2598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="25" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
         <v>60</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="14" t="s">
         <v>60</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="25" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
         <v>58</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
         <v>58</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="28" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="25" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="s">
         <v>58</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="14" t="s">
         <v>58</v>
       </c>
@@ -2713,12 +2713,12 @@
       <selection activeCell="A8" sqref="A8:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="29.83203125" customWidth="1"/>
+    <col min="1" max="5" width="29.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4"/>
       <c r="B1" s="17" t="s">
         <v>56</v>
@@ -2730,7 +2730,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>30</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>34</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>31</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>32</v>
       </c>
@@ -2786,7 +2786,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>33</v>
       </c>
@@ -2800,29 +2800,29 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="41" t="s">
+    <row r="8" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -2843,22 +2843,22 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="3.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="19.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="42" t="s">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C1" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="44"/>
-    </row>
-    <row r="2" spans="1:7" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="47"/>
+    </row>
+    <row r="2" spans="1:7" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="30"/>
       <c r="B2" s="31"/>
       <c r="C2" s="32" t="s">
@@ -2877,8 +2877,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="45" t="s">
+    <row r="3" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="48" t="s">
         <v>47</v>
       </c>
       <c r="B3" s="26" t="s">
@@ -2900,8 +2900,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="46"/>
+    <row r="4" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="49"/>
       <c r="B4" s="34" t="s">
         <v>62</v>
       </c>
@@ -2921,8 +2921,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
+    <row r="5" spans="1:7" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="50"/>
       <c r="B5" s="27" t="s">
         <v>63</v>
       </c>
@@ -2942,8 +2942,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="45" t="s">
+    <row r="6" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="48" t="s">
         <v>45</v>
       </c>
       <c r="B6" s="26" t="s">
@@ -2965,8 +2965,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
+    <row r="7" spans="1:7" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="50"/>
       <c r="B7" s="27" t="s">
         <v>69</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="36" t="s">
         <v>46</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B10" s="23" t="s">
         <v>71</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B11" s="23" t="s">
         <v>72</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B12" s="23" t="s">
         <v>73</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B13" s="23" t="s">
         <v>74</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B14" s="23" t="s">
         <v>75</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B15" s="23" t="s">
         <v>76</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B16" s="23" t="s">
         <v>77</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B17" s="23" t="s">
         <v>78</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B18" s="23" t="s">
         <v>79</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B19" s="23" t="s">
         <v>80</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B20" s="23" t="s">
         <v>81</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B21" s="23" t="s">
         <v>82</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B22" s="23" t="s">
         <v>83</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B23" s="23" t="s">
         <v>84</v>
       </c>
@@ -3121,43 +3121,43 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B24" s="23" t="s">
         <v>85</v>
       </c>
       <c r="C24" s="12"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B25" s="23" t="s">
         <v>86</v>
       </c>
       <c r="C25" s="12"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B26" s="23" t="s">
         <v>87</v>
       </c>
       <c r="C26" s="12"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B27" s="23" t="s">
         <v>88</v>
       </c>
       <c r="C27" s="12"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B28" s="23" t="s">
         <v>89</v>
       </c>
       <c r="C28" s="12"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B29" s="23" t="s">
         <v>90</v>
       </c>
       <c r="C29" s="12"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B30" s="23" t="s">
         <v>91</v>
       </c>
@@ -3182,12 +3182,12 @@
       <selection sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="30.83203125" customWidth="1"/>
+    <col min="1" max="4" width="30.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4"/>
       <c r="B1" s="17" t="s">
         <v>56</v>
@@ -3199,7 +3199,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
         <v>13</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
         <v>14</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="22" t="s">
         <v>39</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
         <v>40</v>
       </c>
@@ -3255,7 +3255,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="22" t="s">
         <v>41</v>
       </c>
@@ -3269,12 +3269,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="41" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B8" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3289,17 +3289,17 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.6328125" customWidth="1"/>
     <col min="2" max="5" width="36" customWidth="1"/>
-    <col min="6" max="6" width="26.6640625" customWidth="1"/>
+    <col min="6" max="6" width="26.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4"/>
       <c r="B1" s="17" t="s">
         <v>93</v>
@@ -3314,253 +3314,253 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="48">
+      <c r="B2" s="40">
         <v>11</v>
       </c>
-      <c r="C2" s="48">
+      <c r="C2" s="40">
         <v>14</v>
       </c>
-      <c r="D2" s="48">
+      <c r="D2" s="40">
         <v>11</v>
       </c>
-      <c r="E2" s="48">
+      <c r="E2" s="40">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="48">
+      <c r="B3" s="40">
         <v>11</v>
       </c>
-      <c r="C3" s="48">
+      <c r="C3" s="40">
         <v>13</v>
       </c>
-      <c r="D3" s="48">
+      <c r="D3" s="40">
         <v>11</v>
       </c>
-      <c r="E3" s="48">
+      <c r="E3" s="40">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="48">
+      <c r="B4" s="40">
         <v>8</v>
       </c>
-      <c r="C4" s="48">
+      <c r="C4" s="40">
         <v>12</v>
       </c>
-      <c r="D4" s="48">
+      <c r="D4" s="40">
         <v>10</v>
       </c>
-      <c r="E4" s="50">
+      <c r="E4" s="42">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="48">
+      <c r="B5" s="40">
         <v>8</v>
       </c>
-      <c r="C5" s="48">
+      <c r="C5" s="40">
         <v>12</v>
       </c>
-      <c r="D5" s="48">
+      <c r="D5" s="40">
         <v>9</v>
       </c>
-      <c r="E5" s="48">
+      <c r="E5" s="40">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="48">
+      <c r="B6" s="40">
         <v>9</v>
       </c>
-      <c r="C6" s="48">
+      <c r="C6" s="40">
         <v>11</v>
       </c>
-      <c r="D6" s="48">
+      <c r="D6" s="40">
         <v>9</v>
       </c>
-      <c r="E6" s="48">
+      <c r="E6" s="40">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="49" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="41" t="s">
         <v>71</v>
       </c>
       <c r="B9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="49" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="41" t="s">
         <v>72</v>
       </c>
       <c r="B10" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="49" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="41" t="s">
         <v>73</v>
       </c>
       <c r="B11" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="49" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="41" t="s">
         <v>74</v>
       </c>
       <c r="B12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="49" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="41" t="s">
         <v>75</v>
       </c>
       <c r="B13" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="49" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="41" t="s">
         <v>76</v>
       </c>
       <c r="B14" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="49" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="41" t="s">
         <v>77</v>
       </c>
       <c r="B15" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="49" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="41" t="s">
         <v>78</v>
       </c>
       <c r="B16" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="49" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="41" t="s">
         <v>79</v>
       </c>
       <c r="B17" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="49" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="41" t="s">
         <v>80</v>
       </c>
       <c r="B18" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="49" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="41" t="s">
         <v>81</v>
       </c>
       <c r="B19" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="49" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="41" t="s">
         <v>82</v>
       </c>
       <c r="B20" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="49" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="41" t="s">
         <v>83</v>
       </c>
       <c r="B21" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="49" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="41" t="s">
         <v>84</v>
       </c>
       <c r="B22" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="49" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="41" t="s">
         <v>85</v>
       </c>
       <c r="B23" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="49" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="41" t="s">
         <v>86</v>
       </c>
       <c r="B24" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="49" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="41" t="s">
         <v>87</v>
       </c>
       <c r="B25" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="49" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="41" t="s">
         <v>88</v>
       </c>
       <c r="B26" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="49" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="41" t="s">
         <v>89</v>
       </c>
       <c r="B27" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="49" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="41" t="s">
         <v>90</v>
       </c>
       <c r="B28" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="49" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="41" t="s">
         <v>91</v>
       </c>
       <c r="B29" t="s">

</xml_diff>

<commit_message>
feat. Feinschliff nicht in Form von Text
</commit_message>
<xml_diff>
--- a/Excel/Mapping Study.xlsx
+++ b/Excel/Mapping Study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bosch-my.sharepoint.com/personal/nnr3fe_bosch_com/Documents/PersonalDrive/HTWG/BA/LaTex/Thesis/Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilsarnold/Documents/WIN-Studium/7. Semester/BA/Thesis/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21382048-7FF6-864D-B436-643A7D7F9E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAD74C7-CECB-6D40-BA98-94607ACEA1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{0DD4CFEA-C2F1-46F7-88F8-AB6F3727EE8E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{0DD4CFEA-C2F1-46F7-88F8-AB6F3727EE8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Zusammenfassung RQ1" sheetId="1" r:id="rId1"/>
@@ -665,7 +665,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -781,11 +781,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1151,16 +1148,16 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.6328125" customWidth="1"/>
-    <col min="2" max="2" width="30.6328125" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
     <col min="3" max="3" width="39" customWidth="1"/>
-    <col min="4" max="4" width="74.6328125" customWidth="1"/>
-    <col min="5" max="5" width="41.1796875" customWidth="1"/>
+    <col min="4" max="4" width="74.6640625" customWidth="1"/>
+    <col min="5" max="5" width="41.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:46" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -1169,8 +1166,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:46" s="4" customFormat="1" ht="51.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="43" t="s">
+    <row r="2" spans="1:46" s="4" customFormat="1" ht="51.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="42" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1225,8 +1222,8 @@
       <c r="AS2"/>
       <c r="AT2"/>
     </row>
-    <row r="3" spans="1:46" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A3" s="43"/>
+    <row r="3" spans="1:46" s="4" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A3" s="42"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1279,8 +1276,8 @@
       <c r="AS3"/>
       <c r="AT3"/>
     </row>
-    <row r="4" spans="1:46" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="43"/>
+    <row r="4" spans="1:46" s="4" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+      <c r="A4" s="42"/>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1333,8 +1330,8 @@
       <c r="AS4"/>
       <c r="AT4"/>
     </row>
-    <row r="5" spans="1:46" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A5" s="43"/>
+    <row r="5" spans="1:46" s="4" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A5" s="42"/>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1387,8 +1384,8 @@
       <c r="AS5"/>
       <c r="AT5"/>
     </row>
-    <row r="6" spans="1:46" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A6" s="43"/>
+    <row r="6" spans="1:46" s="4" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A6" s="42"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1441,8 +1438,8 @@
       <c r="AS6"/>
       <c r="AT6"/>
     </row>
-    <row r="7" spans="1:46" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.35">
-      <c r="A7" s="43" t="s">
+    <row r="7" spans="1:46" s="4" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+      <c r="A7" s="42" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1497,8 +1494,8 @@
       <c r="AS7"/>
       <c r="AT7"/>
     </row>
-    <row r="8" spans="1:46" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="43"/>
+    <row r="8" spans="1:46" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A8" s="42"/>
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1551,8 +1548,8 @@
       <c r="AS8"/>
       <c r="AT8"/>
     </row>
-    <row r="9" spans="1:46" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A9" s="43"/>
+    <row r="9" spans="1:46" s="4" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A9" s="42"/>
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1605,8 +1602,8 @@
       <c r="AS9"/>
       <c r="AT9"/>
     </row>
-    <row r="10" spans="1:46" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A10" s="43"/>
+    <row r="10" spans="1:46" s="4" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A10" s="42"/>
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
@@ -1659,8 +1656,8 @@
       <c r="AS10"/>
       <c r="AT10"/>
     </row>
-    <row r="11" spans="1:46" s="4" customFormat="1" ht="87" x14ac:dyDescent="0.35">
-      <c r="A11" s="43"/>
+    <row r="11" spans="1:46" s="4" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+      <c r="A11" s="42"/>
       <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
@@ -1730,13 +1727,13 @@
       <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.36328125" customWidth="1"/>
-    <col min="2" max="6" width="21.81640625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+    <col min="2" max="6" width="21.83203125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>29</v>
       </c>
@@ -1756,7 +1753,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>30</v>
       </c>
@@ -1776,7 +1773,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>34</v>
       </c>
@@ -1796,7 +1793,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>31</v>
       </c>
@@ -1816,7 +1813,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>32</v>
       </c>
@@ -1836,7 +1833,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>33</v>
       </c>
@@ -1869,17 +1866,17 @@
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.81640625" customWidth="1"/>
-    <col min="2" max="2" width="42.453125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="27.81640625" customWidth="1"/>
-    <col min="4" max="4" width="17.81640625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="19.453125" style="12" customWidth="1"/>
-    <col min="6" max="10" width="21.81640625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="45.83203125" customWidth="1"/>
+    <col min="2" max="2" width="42.5" style="11" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="19.5" style="12" customWidth="1"/>
+    <col min="6" max="10" width="21.83203125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
@@ -1896,7 +1893,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>30</v>
       </c>
@@ -1913,7 +1910,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>30</v>
       </c>
@@ -1931,7 +1928,7 @@
       </c>
       <c r="G3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>30</v>
       </c>
@@ -1949,7 +1946,7 @@
       </c>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>30</v>
       </c>
@@ -1967,7 +1964,7 @@
       </c>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -1985,7 +1982,7 @@
       </c>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>34</v>
       </c>
@@ -2003,7 +2000,7 @@
       </c>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
@@ -2021,7 +2018,7 @@
       </c>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
@@ -2038,7 +2035,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>34</v>
       </c>
@@ -2055,7 +2052,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -2072,7 +2069,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>36</v>
       </c>
@@ -2090,7 +2087,7 @@
       </c>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -2107,7 +2104,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>36</v>
       </c>
@@ -2124,7 +2121,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>36</v>
       </c>
@@ -2141,7 +2138,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>36</v>
       </c>
@@ -2158,7 +2155,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>37</v>
       </c>
@@ -2175,7 +2172,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>37</v>
       </c>
@@ -2192,7 +2189,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>37</v>
       </c>
@@ -2209,7 +2206,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>37</v>
       </c>
@@ -2226,7 +2223,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>37</v>
       </c>
@@ -2243,7 +2240,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>38</v>
       </c>
@@ -2260,7 +2257,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>38</v>
       </c>
@@ -2277,7 +2274,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>38</v>
       </c>
@@ -2294,7 +2291,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>38</v>
       </c>
@@ -2311,7 +2308,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>38</v>
       </c>
@@ -2338,18 +2335,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01DF9B60-2E89-4293-8875-39A769A4224F}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="4" width="23.81640625" customWidth="1"/>
-    <col min="7" max="10" width="26.1796875" customWidth="1"/>
+    <col min="2" max="4" width="23.83203125" customWidth="1"/>
+    <col min="7" max="10" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>44</v>
       </c>
@@ -2375,7 +2372,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>48</v>
       </c>
@@ -2383,10 +2380,10 @@
         <v>14</v>
       </c>
       <c r="C2" s="2">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>48</v>
@@ -2401,7 +2398,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>49</v>
       </c>
@@ -2427,7 +2424,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>50</v>
       </c>
@@ -2453,7 +2450,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>51</v>
       </c>
@@ -2461,7 +2458,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
@@ -2479,7 +2476,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>64</v>
       </c>
@@ -2496,7 +2493,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="28" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>56</v>
       </c>
@@ -2513,7 +2510,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>59</v>
       </c>
@@ -2530,7 +2527,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="28" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>56</v>
       </c>
@@ -2547,7 +2544,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>59</v>
       </c>
@@ -2564,7 +2561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="28" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>60</v>
       </c>
@@ -2581,7 +2578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>60</v>
       </c>
@@ -2598,7 +2595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="28" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>60</v>
       </c>
@@ -2615,7 +2612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>60</v>
       </c>
@@ -2632,7 +2629,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="28" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>58</v>
       </c>
@@ -2649,7 +2646,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>58</v>
       </c>
@@ -2666,7 +2663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="25" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="28" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>58</v>
       </c>
@@ -2683,7 +2680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>58</v>
       </c>
@@ -2713,12 +2710,12 @@
       <selection activeCell="A8" sqref="A8:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="29.81640625" customWidth="1"/>
+    <col min="1" max="5" width="29.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="17" t="s">
         <v>56</v>
@@ -2730,7 +2727,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
         <v>30</v>
       </c>
@@ -2744,7 +2741,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
         <v>34</v>
       </c>
@@ -2758,7 +2755,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
         <v>31</v>
       </c>
@@ -2772,7 +2769,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
         <v>32</v>
       </c>
@@ -2786,7 +2783,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
         <v>33</v>
       </c>
@@ -2800,29 +2797,29 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="44" t="s">
+    <row r="8" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -2843,22 +2840,22 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="19.6328125" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="45" t="s">
+    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="47"/>
-    </row>
-    <row r="2" spans="1:7" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="46"/>
+    </row>
+    <row r="2" spans="1:7" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30"/>
       <c r="B2" s="31"/>
       <c r="C2" s="32" t="s">
@@ -2877,8 +2874,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="48" t="s">
+    <row r="3" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="47" t="s">
         <v>47</v>
       </c>
       <c r="B3" s="26" t="s">
@@ -2900,8 +2897,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="49"/>
+    <row r="4" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="48"/>
       <c r="B4" s="34" t="s">
         <v>62</v>
       </c>
@@ -2921,8 +2918,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="50"/>
+    <row r="5" spans="1:7" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="49"/>
       <c r="B5" s="27" t="s">
         <v>63</v>
       </c>
@@ -2942,8 +2939,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="48" t="s">
+    <row r="6" spans="1:7" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="47" t="s">
         <v>45</v>
       </c>
       <c r="B6" s="26" t="s">
@@ -2965,8 +2962,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="50"/>
+    <row r="7" spans="1:7" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="49"/>
       <c r="B7" s="27" t="s">
         <v>69</v>
       </c>
@@ -2986,7 +2983,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>46</v>
       </c>
@@ -3009,7 +3006,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B10" s="23" t="s">
         <v>71</v>
       </c>
@@ -3017,7 +3014,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" s="23" t="s">
         <v>72</v>
       </c>
@@ -3025,7 +3022,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="23" t="s">
         <v>73</v>
       </c>
@@ -3033,7 +3030,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" s="23" t="s">
         <v>74</v>
       </c>
@@ -3041,7 +3038,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" s="23" t="s">
         <v>75</v>
       </c>
@@ -3049,7 +3046,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" s="23" t="s">
         <v>76</v>
       </c>
@@ -3057,7 +3054,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" s="23" t="s">
         <v>77</v>
       </c>
@@ -3065,7 +3062,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="23" t="s">
         <v>78</v>
       </c>
@@ -3073,7 +3070,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="23" t="s">
         <v>79</v>
       </c>
@@ -3081,7 +3078,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="23" t="s">
         <v>80</v>
       </c>
@@ -3089,7 +3086,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="23" t="s">
         <v>81</v>
       </c>
@@ -3097,7 +3094,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="23" t="s">
         <v>82</v>
       </c>
@@ -3105,7 +3102,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="23" t="s">
         <v>83</v>
       </c>
@@ -3113,7 +3110,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="23" t="s">
         <v>84</v>
       </c>
@@ -3121,43 +3118,43 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" s="23" t="s">
         <v>85</v>
       </c>
       <c r="C24" s="12"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" s="23" t="s">
         <v>86</v>
       </c>
       <c r="C25" s="12"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B26" s="23" t="s">
         <v>87</v>
       </c>
       <c r="C26" s="12"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B27" s="23" t="s">
         <v>88</v>
       </c>
       <c r="C27" s="12"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B28" s="23" t="s">
         <v>89</v>
       </c>
       <c r="C28" s="12"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B29" s="23" t="s">
         <v>90</v>
       </c>
       <c r="C29" s="12"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B30" s="23" t="s">
         <v>91</v>
       </c>
@@ -3182,12 +3179,12 @@
       <selection sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="30.81640625" customWidth="1"/>
+    <col min="1" max="4" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="17" t="s">
         <v>56</v>
@@ -3199,7 +3196,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
         <v>13</v>
       </c>
@@ -3213,7 +3210,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
         <v>14</v>
       </c>
@@ -3227,7 +3224,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
         <v>39</v>
       </c>
@@ -3241,7 +3238,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
         <v>40</v>
       </c>
@@ -3255,7 +3252,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
         <v>41</v>
       </c>
@@ -3269,12 +3266,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B8" s="44" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3288,18 +3285,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08D85E9E-A320-8846-8F2A-00C580DDC52A}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+    <sheetView zoomScale="83" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.6328125" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" customWidth="1"/>
     <col min="2" max="5" width="36" customWidth="1"/>
-    <col min="6" max="6" width="26.6328125" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="17" t="s">
         <v>93</v>
@@ -3314,7 +3311,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
         <v>13</v>
       </c>
@@ -3331,7 +3328,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
         <v>14</v>
       </c>
@@ -3348,7 +3345,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
         <v>39</v>
       </c>
@@ -3361,11 +3358,11 @@
       <c r="D4" s="40">
         <v>10</v>
       </c>
-      <c r="E4" s="42">
+      <c r="E4" s="40">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
         <v>40</v>
       </c>
@@ -3382,7 +3379,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
         <v>41</v>
       </c>
@@ -3399,7 +3396,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="41" t="s">
         <v>71</v>
       </c>
@@ -3407,7 +3404,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="41" t="s">
         <v>72</v>
       </c>
@@ -3415,7 +3412,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="41" t="s">
         <v>73</v>
       </c>
@@ -3423,7 +3420,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="41" t="s">
         <v>74</v>
       </c>
@@ -3431,7 +3428,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="41" t="s">
         <v>75</v>
       </c>
@@ -3439,7 +3436,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="41" t="s">
         <v>76</v>
       </c>
@@ -3447,7 +3444,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="41" t="s">
         <v>77</v>
       </c>
@@ -3455,7 +3452,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="41" t="s">
         <v>78</v>
       </c>
@@ -3463,7 +3460,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="41" t="s">
         <v>79</v>
       </c>
@@ -3471,7 +3468,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="41" t="s">
         <v>80</v>
       </c>
@@ -3479,7 +3476,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="41" t="s">
         <v>81</v>
       </c>
@@ -3487,7 +3484,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="41" t="s">
         <v>82</v>
       </c>
@@ -3495,7 +3492,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="41" t="s">
         <v>83</v>
       </c>
@@ -3503,7 +3500,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="41" t="s">
         <v>84</v>
       </c>
@@ -3511,7 +3508,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="41" t="s">
         <v>85</v>
       </c>
@@ -3519,7 +3516,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="41" t="s">
         <v>86</v>
       </c>
@@ -3527,7 +3524,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="41" t="s">
         <v>87</v>
       </c>
@@ -3535,7 +3532,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="41" t="s">
         <v>88</v>
       </c>
@@ -3543,7 +3540,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="41" t="s">
         <v>89</v>
       </c>
@@ -3551,7 +3548,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="41" t="s">
         <v>90</v>
       </c>
@@ -3559,7 +3556,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="41" t="s">
         <v>91</v>
       </c>

</xml_diff>